<commit_message>
add: create URDF files to generate first WOI to optimiziation
</commit_message>
<xml_diff>
--- a/general/concepts/left_concepts.xlsx
+++ b/general/concepts/left_concepts.xlsx
@@ -82,6 +82,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -177,22 +178,22 @@
   </sheetPr>
   <dimension ref="A1:J795"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A597" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J351" activeCellId="0" sqref="J351:J611"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="4.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.42"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="11" style="1" width="11.52"/>
   </cols>
   <sheetData>
@@ -11422,10 +11423,10 @@
         <v>220</v>
       </c>
       <c r="I351" s="1" t="n">
-        <v>28</v>
+        <v>220</v>
       </c>
       <c r="J351" s="1" t="n">
-        <v>192</v>
+        <v>0</v>
       </c>
     </row>
     <row r="352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11454,10 +11455,10 @@
         <v>220</v>
       </c>
       <c r="I352" s="1" t="n">
-        <v>27</v>
+        <v>220</v>
       </c>
       <c r="J352" s="1" t="n">
-        <v>193</v>
+        <v>0</v>
       </c>
     </row>
     <row r="353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11486,10 +11487,10 @@
         <v>220</v>
       </c>
       <c r="I353" s="1" t="n">
-        <v>31</v>
+        <v>220</v>
       </c>
       <c r="J353" s="1" t="n">
-        <v>189</v>
+        <v>0</v>
       </c>
     </row>
     <row r="354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11518,10 +11519,10 @@
         <v>220</v>
       </c>
       <c r="I354" s="1" t="n">
-        <v>33</v>
+        <v>220</v>
       </c>
       <c r="J354" s="1" t="n">
-        <v>187</v>
+        <v>0</v>
       </c>
     </row>
     <row r="355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11550,10 +11551,10 @@
         <v>220</v>
       </c>
       <c r="I355" s="1" t="n">
-        <v>31</v>
+        <v>220</v>
       </c>
       <c r="J355" s="1" t="n">
-        <v>189</v>
+        <v>0</v>
       </c>
     </row>
     <row r="356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11742,10 +11743,10 @@
         <v>225</v>
       </c>
       <c r="I361" s="1" t="n">
-        <v>29</v>
+        <v>225</v>
       </c>
       <c r="J361" s="1" t="n">
-        <v>196</v>
+        <v>0</v>
       </c>
     </row>
     <row r="362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11774,10 +11775,10 @@
         <v>225</v>
       </c>
       <c r="I362" s="1" t="n">
-        <v>26</v>
+        <v>225</v>
       </c>
       <c r="J362" s="1" t="n">
-        <v>199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11902,10 +11903,10 @@
         <v>228</v>
       </c>
       <c r="I366" s="1" t="n">
-        <v>47</v>
+        <v>228</v>
       </c>
       <c r="J366" s="1" t="n">
-        <v>181</v>
+        <v>0</v>
       </c>
     </row>
     <row r="367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11934,10 +11935,10 @@
         <v>231</v>
       </c>
       <c r="I367" s="1" t="n">
-        <v>29</v>
+        <v>231</v>
       </c>
       <c r="J367" s="1" t="n">
-        <v>202</v>
+        <v>0</v>
       </c>
     </row>
     <row r="368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11998,10 +11999,10 @@
         <v>240</v>
       </c>
       <c r="I369" s="1" t="n">
-        <v>32</v>
+        <v>239</v>
       </c>
       <c r="J369" s="1" t="n">
-        <v>208</v>
+        <v>1</v>
       </c>
     </row>
     <row r="370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12094,10 +12095,10 @@
         <v>240</v>
       </c>
       <c r="I372" s="1" t="n">
-        <v>33</v>
+        <v>240</v>
       </c>
       <c r="J372" s="1" t="n">
-        <v>207</v>
+        <v>0</v>
       </c>
     </row>
     <row r="373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12126,10 +12127,10 @@
         <v>240</v>
       </c>
       <c r="I373" s="1" t="n">
-        <v>29</v>
+        <v>240</v>
       </c>
       <c r="J373" s="1" t="n">
-        <v>211</v>
+        <v>0</v>
       </c>
     </row>
     <row r="374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12158,10 +12159,10 @@
         <v>247</v>
       </c>
       <c r="I374" s="1" t="n">
-        <v>76</v>
+        <v>247</v>
       </c>
       <c r="J374" s="1" t="n">
-        <v>171</v>
+        <v>0</v>
       </c>
     </row>
     <row r="375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12190,10 +12191,10 @@
         <v>250</v>
       </c>
       <c r="I375" s="1" t="n">
-        <v>27</v>
+        <v>250</v>
       </c>
       <c r="J375" s="1" t="n">
-        <v>223</v>
+        <v>0</v>
       </c>
     </row>
     <row r="376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12350,10 +12351,10 @@
         <v>260</v>
       </c>
       <c r="I380" s="1" t="n">
-        <v>26</v>
+        <v>260</v>
       </c>
       <c r="J380" s="1" t="n">
-        <v>234</v>
+        <v>0</v>
       </c>
     </row>
     <row r="381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12382,10 +12383,10 @@
         <v>260</v>
       </c>
       <c r="I381" s="1" t="n">
-        <v>34</v>
+        <v>260</v>
       </c>
       <c r="J381" s="1" t="n">
-        <v>226</v>
+        <v>0</v>
       </c>
     </row>
     <row r="382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12414,10 +12415,10 @@
         <v>260</v>
       </c>
       <c r="I382" s="1" t="n">
-        <v>30</v>
+        <v>260</v>
       </c>
       <c r="J382" s="1" t="n">
-        <v>230</v>
+        <v>0</v>
       </c>
     </row>
     <row r="383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12446,10 +12447,10 @@
         <v>260</v>
       </c>
       <c r="I383" s="1" t="n">
-        <v>30</v>
+        <v>260</v>
       </c>
       <c r="J383" s="1" t="n">
-        <v>230</v>
+        <v>0</v>
       </c>
     </row>
     <row r="384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12478,10 +12479,10 @@
         <v>260</v>
       </c>
       <c r="I384" s="1" t="n">
-        <v>31</v>
+        <v>260</v>
       </c>
       <c r="J384" s="1" t="n">
-        <v>229</v>
+        <v>0</v>
       </c>
     </row>
     <row r="385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12510,10 +12511,10 @@
         <v>260</v>
       </c>
       <c r="I385" s="1" t="n">
-        <v>30</v>
+        <v>260</v>
       </c>
       <c r="J385" s="1" t="n">
-        <v>230</v>
+        <v>0</v>
       </c>
     </row>
     <row r="386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12542,10 +12543,10 @@
         <v>260</v>
       </c>
       <c r="I386" s="1" t="n">
-        <v>30</v>
+        <v>260</v>
       </c>
       <c r="J386" s="1" t="n">
-        <v>230</v>
+        <v>0</v>
       </c>
     </row>
     <row r="387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12574,10 +12575,10 @@
         <v>260</v>
       </c>
       <c r="I387" s="1" t="n">
-        <v>31</v>
+        <v>260</v>
       </c>
       <c r="J387" s="1" t="n">
-        <v>229</v>
+        <v>0</v>
       </c>
     </row>
     <row r="388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12606,10 +12607,10 @@
         <v>260</v>
       </c>
       <c r="I388" s="1" t="n">
-        <v>28</v>
+        <v>260</v>
       </c>
       <c r="J388" s="1" t="n">
-        <v>232</v>
+        <v>0</v>
       </c>
     </row>
     <row r="389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12638,10 +12639,10 @@
         <v>264</v>
       </c>
       <c r="I389" s="1" t="n">
-        <v>52</v>
+        <v>264</v>
       </c>
       <c r="J389" s="1" t="n">
-        <v>212</v>
+        <v>0</v>
       </c>
     </row>
     <row r="390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12670,10 +12671,10 @@
         <v>264</v>
       </c>
       <c r="I390" s="1" t="n">
-        <v>33</v>
+        <v>264</v>
       </c>
       <c r="J390" s="1" t="n">
-        <v>231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12702,10 +12703,10 @@
         <v>264</v>
       </c>
       <c r="I391" s="1" t="n">
-        <v>29</v>
+        <v>263</v>
       </c>
       <c r="J391" s="1" t="n">
-        <v>235</v>
+        <v>1</v>
       </c>
     </row>
     <row r="392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12734,10 +12735,10 @@
         <v>264</v>
       </c>
       <c r="I392" s="1" t="n">
-        <v>29</v>
+        <v>264</v>
       </c>
       <c r="J392" s="1" t="n">
-        <v>235</v>
+        <v>0</v>
       </c>
     </row>
     <row r="393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12766,10 +12767,10 @@
         <v>266</v>
       </c>
       <c r="I393" s="1" t="n">
-        <v>37</v>
+        <v>265</v>
       </c>
       <c r="J393" s="1" t="n">
-        <v>229</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12798,10 +12799,10 @@
         <v>270</v>
       </c>
       <c r="I394" s="1" t="n">
-        <v>56</v>
+        <v>270</v>
       </c>
       <c r="J394" s="1" t="n">
-        <v>214</v>
+        <v>0</v>
       </c>
     </row>
     <row r="395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12862,10 +12863,10 @@
         <v>280</v>
       </c>
       <c r="I396" s="1" t="n">
-        <v>31</v>
+        <v>280</v>
       </c>
       <c r="J396" s="1" t="n">
-        <v>249</v>
+        <v>0</v>
       </c>
     </row>
     <row r="397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12894,10 +12895,10 @@
         <v>280</v>
       </c>
       <c r="I397" s="1" t="n">
-        <v>29</v>
+        <v>280</v>
       </c>
       <c r="J397" s="1" t="n">
-        <v>251</v>
+        <v>0</v>
       </c>
     </row>
     <row r="398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12926,10 +12927,10 @@
         <v>284</v>
       </c>
       <c r="I398" s="1" t="n">
-        <v>35</v>
+        <v>284</v>
       </c>
       <c r="J398" s="1" t="n">
-        <v>249</v>
+        <v>0</v>
       </c>
     </row>
     <row r="399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12958,10 +12959,10 @@
         <v>284</v>
       </c>
       <c r="I399" s="1" t="n">
-        <v>32</v>
+        <v>284</v>
       </c>
       <c r="J399" s="1" t="n">
-        <v>252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12990,10 +12991,10 @@
         <v>286</v>
       </c>
       <c r="I400" s="1" t="n">
-        <v>34</v>
+        <v>286</v>
       </c>
       <c r="J400" s="1" t="n">
-        <v>252</v>
+        <v>0</v>
       </c>
     </row>
     <row r="401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13118,10 +13119,10 @@
         <v>295</v>
       </c>
       <c r="I404" s="1" t="n">
-        <v>33</v>
+        <v>294</v>
       </c>
       <c r="J404" s="1" t="n">
-        <v>262</v>
+        <v>1</v>
       </c>
     </row>
     <row r="405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13150,10 +13151,10 @@
         <v>295</v>
       </c>
       <c r="I405" s="1" t="n">
-        <v>31</v>
+        <v>295</v>
       </c>
       <c r="J405" s="1" t="n">
-        <v>264</v>
+        <v>0</v>
       </c>
     </row>
     <row r="406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13182,10 +13183,10 @@
         <v>300</v>
       </c>
       <c r="I406" s="1" t="n">
-        <v>30</v>
+        <v>300</v>
       </c>
       <c r="J406" s="1" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13278,10 +13279,10 @@
         <v>308</v>
       </c>
       <c r="I409" s="1" t="n">
-        <v>35</v>
+        <v>308</v>
       </c>
       <c r="J409" s="1" t="n">
-        <v>273</v>
+        <v>0</v>
       </c>
     </row>
     <row r="410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13342,10 +13343,10 @@
         <v>325</v>
       </c>
       <c r="I411" s="1" t="n">
-        <v>31</v>
+        <v>325</v>
       </c>
       <c r="J411" s="1" t="n">
-        <v>294</v>
+        <v>0</v>
       </c>
     </row>
     <row r="412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13374,10 +13375,10 @@
         <v>330</v>
       </c>
       <c r="I412" s="1" t="n">
-        <v>29</v>
+        <v>330</v>
       </c>
       <c r="J412" s="1" t="n">
-        <v>301</v>
+        <v>0</v>
       </c>
     </row>
     <row r="413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13406,10 +13407,10 @@
         <v>336</v>
       </c>
       <c r="I413" s="1" t="n">
-        <v>66</v>
+        <v>336</v>
       </c>
       <c r="J413" s="1" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13438,10 +13439,10 @@
         <v>342</v>
       </c>
       <c r="I414" s="1" t="n">
-        <v>109</v>
+        <v>342</v>
       </c>
       <c r="J414" s="1" t="n">
-        <v>233</v>
+        <v>0</v>
       </c>
     </row>
     <row r="415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13470,10 +13471,10 @@
         <v>350</v>
       </c>
       <c r="I415" s="1" t="n">
-        <v>32</v>
+        <v>350</v>
       </c>
       <c r="J415" s="1" t="n">
-        <v>318</v>
+        <v>0</v>
       </c>
     </row>
     <row r="416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13502,10 +13503,10 @@
         <v>354</v>
       </c>
       <c r="I416" s="1" t="n">
-        <v>36</v>
+        <v>353</v>
       </c>
       <c r="J416" s="1" t="n">
-        <v>318</v>
+        <v>1</v>
       </c>
     </row>
     <row r="417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13566,10 +13567,10 @@
         <v>380</v>
       </c>
       <c r="I418" s="1" t="n">
-        <v>31</v>
+        <v>380</v>
       </c>
       <c r="J418" s="1" t="n">
-        <v>349</v>
+        <v>0</v>
       </c>
     </row>
     <row r="419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13630,10 +13631,10 @@
         <v>380</v>
       </c>
       <c r="I420" s="1" t="n">
-        <v>34</v>
+        <v>380</v>
       </c>
       <c r="J420" s="1" t="n">
-        <v>346</v>
+        <v>0</v>
       </c>
     </row>
     <row r="421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13662,10 +13663,10 @@
         <v>380</v>
       </c>
       <c r="I421" s="1" t="n">
-        <v>33</v>
+        <v>380</v>
       </c>
       <c r="J421" s="1" t="n">
-        <v>347</v>
+        <v>0</v>
       </c>
     </row>
     <row r="422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13758,10 +13759,10 @@
         <v>390</v>
       </c>
       <c r="I424" s="1" t="n">
-        <v>35</v>
+        <v>390</v>
       </c>
       <c r="J424" s="1" t="n">
-        <v>355</v>
+        <v>0</v>
       </c>
     </row>
     <row r="425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13790,10 +13791,10 @@
         <v>396</v>
       </c>
       <c r="I425" s="1" t="n">
-        <v>34</v>
+        <v>396</v>
       </c>
       <c r="J425" s="1" t="n">
-        <v>362</v>
+        <v>0</v>
       </c>
     </row>
     <row r="426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13918,10 +13919,10 @@
         <v>420</v>
       </c>
       <c r="I429" s="1" t="n">
-        <v>36</v>
+        <v>420</v>
       </c>
       <c r="J429" s="1" t="n">
-        <v>384</v>
+        <v>0</v>
       </c>
     </row>
     <row r="430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13950,10 +13951,10 @@
         <v>420</v>
       </c>
       <c r="I430" s="1" t="n">
-        <v>34</v>
+        <v>419</v>
       </c>
       <c r="J430" s="1" t="n">
-        <v>386</v>
+        <v>1</v>
       </c>
     </row>
     <row r="431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13982,10 +13983,10 @@
         <v>429</v>
       </c>
       <c r="I431" s="1" t="n">
-        <v>34</v>
+        <v>429</v>
       </c>
       <c r="J431" s="1" t="n">
-        <v>395</v>
+        <v>0</v>
       </c>
     </row>
     <row r="432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14014,10 +14015,10 @@
         <v>430</v>
       </c>
       <c r="I432" s="1" t="n">
-        <v>31</v>
+        <v>430</v>
       </c>
       <c r="J432" s="1" t="n">
-        <v>399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14046,10 +14047,10 @@
         <v>430</v>
       </c>
       <c r="I433" s="1" t="n">
-        <v>31</v>
+        <v>428</v>
       </c>
       <c r="J433" s="1" t="n">
-        <v>399</v>
+        <v>2</v>
       </c>
     </row>
     <row r="434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14110,10 +14111,10 @@
         <v>440</v>
       </c>
       <c r="I435" s="1" t="n">
-        <v>32</v>
+        <v>440</v>
       </c>
       <c r="J435" s="1" t="n">
-        <v>408</v>
+        <v>0</v>
       </c>
     </row>
     <row r="436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14142,10 +14143,10 @@
         <v>440</v>
       </c>
       <c r="I436" s="1" t="n">
-        <v>30</v>
+        <v>439</v>
       </c>
       <c r="J436" s="1" t="n">
-        <v>410</v>
+        <v>1</v>
       </c>
     </row>
     <row r="437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14174,10 +14175,10 @@
         <v>440</v>
       </c>
       <c r="I437" s="1" t="n">
-        <v>34</v>
+        <v>440</v>
       </c>
       <c r="J437" s="1" t="n">
-        <v>406</v>
+        <v>0</v>
       </c>
     </row>
     <row r="438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14206,10 +14207,10 @@
         <v>440</v>
       </c>
       <c r="I438" s="1" t="n">
-        <v>37</v>
+        <v>440</v>
       </c>
       <c r="J438" s="1" t="n">
-        <v>403</v>
+        <v>0</v>
       </c>
     </row>
     <row r="439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14238,10 +14239,10 @@
         <v>440</v>
       </c>
       <c r="I439" s="1" t="n">
-        <v>35</v>
+        <v>439</v>
       </c>
       <c r="J439" s="1" t="n">
-        <v>405</v>
+        <v>1</v>
       </c>
     </row>
     <row r="440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14270,10 +14271,10 @@
         <v>440</v>
       </c>
       <c r="I440" s="1" t="n">
-        <v>32</v>
+        <v>440</v>
       </c>
       <c r="J440" s="1" t="n">
-        <v>408</v>
+        <v>0</v>
       </c>
     </row>
     <row r="441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14366,10 +14367,10 @@
         <v>450</v>
       </c>
       <c r="I443" s="1" t="n">
-        <v>35</v>
+        <v>449</v>
       </c>
       <c r="J443" s="1" t="n">
-        <v>415</v>
+        <v>1</v>
       </c>
     </row>
     <row r="444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14398,10 +14399,10 @@
         <v>450</v>
       </c>
       <c r="I444" s="1" t="n">
-        <v>35</v>
+        <v>450</v>
       </c>
       <c r="J444" s="1" t="n">
-        <v>415</v>
+        <v>0</v>
       </c>
     </row>
     <row r="445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14430,10 +14431,10 @@
         <v>450</v>
       </c>
       <c r="I445" s="1" t="n">
-        <v>30</v>
+        <v>450</v>
       </c>
       <c r="J445" s="1" t="n">
-        <v>420</v>
+        <v>0</v>
       </c>
     </row>
     <row r="446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14462,10 +14463,10 @@
         <v>450</v>
       </c>
       <c r="I446" s="1" t="n">
-        <v>32</v>
+        <v>450</v>
       </c>
       <c r="J446" s="1" t="n">
-        <v>418</v>
+        <v>0</v>
       </c>
     </row>
     <row r="447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14494,10 +14495,10 @@
         <v>462</v>
       </c>
       <c r="I447" s="1" t="n">
-        <v>34</v>
+        <v>462</v>
       </c>
       <c r="J447" s="1" t="n">
-        <v>428</v>
+        <v>0</v>
       </c>
     </row>
     <row r="448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14622,10 +14623,10 @@
         <v>480</v>
       </c>
       <c r="I451" s="1" t="n">
-        <v>34</v>
+        <v>480</v>
       </c>
       <c r="J451" s="1" t="n">
-        <v>446</v>
+        <v>0</v>
       </c>
     </row>
     <row r="452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14654,10 +14655,10 @@
         <v>480</v>
       </c>
       <c r="I452" s="1" t="n">
-        <v>40</v>
+        <v>480</v>
       </c>
       <c r="J452" s="1" t="n">
-        <v>440</v>
+        <v>0</v>
       </c>
     </row>
     <row r="453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14686,10 +14687,10 @@
         <v>494</v>
       </c>
       <c r="I453" s="1" t="n">
-        <v>61</v>
+        <v>494</v>
       </c>
       <c r="J453" s="1" t="n">
-        <v>433</v>
+        <v>0</v>
       </c>
     </row>
     <row r="454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14718,10 +14719,10 @@
         <v>494</v>
       </c>
       <c r="I454" s="1" t="n">
-        <v>32</v>
+        <v>494</v>
       </c>
       <c r="J454" s="1" t="n">
-        <v>462</v>
+        <v>0</v>
       </c>
     </row>
     <row r="455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14750,10 +14751,10 @@
         <v>494</v>
       </c>
       <c r="I455" s="1" t="n">
-        <v>54</v>
+        <v>493</v>
       </c>
       <c r="J455" s="1" t="n">
-        <v>440</v>
+        <v>1</v>
       </c>
     </row>
     <row r="456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14782,10 +14783,10 @@
         <v>495</v>
       </c>
       <c r="I456" s="1" t="n">
-        <v>34</v>
+        <v>495</v>
       </c>
       <c r="J456" s="1" t="n">
-        <v>461</v>
+        <v>0</v>
       </c>
     </row>
     <row r="457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14814,10 +14815,10 @@
         <v>495</v>
       </c>
       <c r="I457" s="1" t="n">
-        <v>39</v>
+        <v>495</v>
       </c>
       <c r="J457" s="1" t="n">
-        <v>456</v>
+        <v>0</v>
       </c>
     </row>
     <row r="458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>